<commit_message>
added inorganic carbon data
</commit_message>
<xml_diff>
--- a/BD for HH and PS.xlsx
+++ b/BD for HH and PS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F004SPC\Documents\GitHub\FracFarmVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f004spc\Documents\GitHub\FracFarmVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2CB1513-0499-4661-9F7D-6378B7F571C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411B568B-4A0C-4961-8883-46CD553A4AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E2507CA8-1A4E-4C71-9738-47144C21E4CF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>HH28</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>dry plus tin</t>
+  </si>
+  <si>
+    <t>UD</t>
+  </si>
+  <si>
+    <t>LD</t>
   </si>
 </sst>
 </file>
@@ -440,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C30B34-2E29-42E2-9B9C-AC5556C4C1AA}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -464,8 +470,14 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -485,7 +497,7 @@
         <v>11.177300000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -505,7 +517,7 @@
         <v>16.094000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -525,7 +537,7 @@
         <v>15.0488</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -545,7 +557,7 @@
         <v>25.985900000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>

</xml_diff>